<commit_message>
Add goods and services data from H24
</commit_message>
<xml_diff>
--- a/data/goods_services/h23_youshiki3-4.xlsx
+++ b/data/goods_services/h23_youshiki3-4.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorincerti/Documents/GitHub/jNPO/data/goods_services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C387D147-1B8B-5942-AC02-36933AAC486E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BED1BA4-2118-DD4D-9C1D-8A0C750432E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">sheet1!$A$1:$P$737</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">sheet1!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8800" uniqueCount="1853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8798" uniqueCount="1851">
   <si>
     <t>契約を締結した日</t>
     <rPh sb="0" eb="2">
@@ -23936,27 +23936,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>単価契約
-単価のみ</t>
-    <rPh sb="0" eb="2">
-      <t>タンカ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>タンカ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ドル払い</t>
-    <rPh sb="2" eb="3">
-      <t>バラ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>共同企業体代表者　社団法人海外林業コンサルタンツ協会
 東京都文京区本郷2-38-4 本郷弓町ﾋﾞﾙ3F
 構成員　一般社団法人日本森林技術協会</t>
@@ -24202,20 +24181,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="12">
     <numFmt numFmtId="164" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[$-411]ggge&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="177" formatCode="#,##0_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0;&quot;△ &quot;#,##0"/>
-    <numFmt numFmtId="179" formatCode="#,##0&quot;円&quot;"/>
-    <numFmt numFmtId="180" formatCode="#,##0_ ;__\ &quot;△&quot;* #,##0_ ;&quot;－&quot;_ ;@"/>
-    <numFmt numFmtId="181" formatCode="#,##0_ ;__\ &quot;△&quot;* #,##0_ ;[Color15]&quot;－&quot;_ ;@"/>
-    <numFmt numFmtId="182" formatCode="#,##0&quot;人&quot;"/>
-    <numFmt numFmtId="183" formatCode="0;&quot;△ &quot;0"/>
-    <numFmt numFmtId="184" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="[$-411]ggge&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="168" formatCode="#,##0_ "/>
+    <numFmt numFmtId="169" formatCode="#,##0;&quot;△ &quot;#,##0"/>
+    <numFmt numFmtId="170" formatCode="#,##0&quot;円&quot;"/>
+    <numFmt numFmtId="171" formatCode="#,##0_ ;__\ &quot;△&quot;* #,##0_ ;&quot;－&quot;_ ;@"/>
+    <numFmt numFmtId="172" formatCode="#,##0_ ;__\ &quot;△&quot;* #,##0_ ;[Color15]&quot;－&quot;_ ;@"/>
+    <numFmt numFmtId="173" formatCode="#,##0&quot;人&quot;"/>
+    <numFmt numFmtId="174" formatCode="0;&quot;△ &quot;0"/>
+    <numFmt numFmtId="175" formatCode="0.0%"/>
   </numFmts>
   <fonts count="50">
     <font>
@@ -24656,7 +24635,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -24690,10 +24669,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24702,7 +24681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24735,7 +24714,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24744,10 +24723,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24756,16 +24735,16 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="181" fontId="36" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="36" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24780,7 +24759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24807,7 +24786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24828,16 +24807,16 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24849,7 +24828,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24858,7 +24837,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24867,7 +24846,7 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24876,7 +24855,7 @@
     <xf numFmtId="38" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24975,55 +24954,55 @@
     <xf numFmtId="14" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="38" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="38" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25032,7 +25011,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="40" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="40" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="37" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25047,13 +25026,13 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="184" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25071,7 +25050,7 @@
     <xf numFmtId="38" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="38" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25080,7 +25059,7 @@
     <xf numFmtId="38" fontId="36" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25089,7 +25068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25098,7 +25077,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="36" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25125,16 +25104,16 @@
     <xf numFmtId="38" fontId="37" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="36" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25149,13 +25128,13 @@
     <xf numFmtId="38" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25173,7 +25152,7 @@
     <xf numFmtId="37" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25188,7 +25167,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25197,7 +25176,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="37" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25209,7 +25188,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25218,7 +25197,7 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -25233,7 +25212,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="37" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="37" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
@@ -25245,7 +25224,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="36" fillId="0" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25257,19 +25236,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25296,7 +25275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="35" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="175" fontId="35" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="47" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25313,9 +25292,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -25374,22 +25350,22 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="175" fontId="36" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="175" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25422,10 +25398,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -25446,19 +25422,19 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="桁区切り 2" xfId="3"/>
-    <cellStyle name="標準 2" xfId="5"/>
-    <cellStyle name="標準 4" xfId="6"/>
-    <cellStyle name="標準 5" xfId="7"/>
-    <cellStyle name="標準 6" xfId="8"/>
-    <cellStyle name="標準 6 2" xfId="9"/>
-    <cellStyle name="標準_【フォーム】契約csvフォーマット" xfId="10"/>
-    <cellStyle name="標準_【委託⑱】１8年度契約締結分" xfId="11"/>
-    <cellStyle name="標準_１６７調査票４案件best100（再検討）0914提出用" xfId="12"/>
-    <cellStyle name="標準_公表資料枠組み(H20.7.22最新）" xfId="13"/>
-    <cellStyle name="標準_公表資料枠組み(H20.7.22最新） 2" xfId="14"/>
-    <cellStyle name="標準_別添１・２（請求計画表・工事一覧表）" xfId="16"/>
-    <cellStyle name="標準_随意契約1月" xfId="15"/>
+    <cellStyle name="桁区切り 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="標準 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="標準 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="標準 6" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="標準 6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="標準_【フォーム】契約csvフォーマット" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="標準_【委託⑱】１8年度契約締結分" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="標準_１６７調査票４案件best100（再検討）0914提出用" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="標準_公表資料枠組み(H20.7.22最新）" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="標準_公表資料枠組み(H20.7.22最新） 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="標準_別添１・２（請求計画表・工事一覧表）" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="標準_随意契約1月" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -25793,11 +25769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V737"/>
+  <dimension ref="A1:U737"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -25824,72 +25800,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A1" s="260" t="s">
-        <v>1847</v>
-      </c>
-      <c r="B1" s="260"/>
-      <c r="C1" s="260"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
-      <c r="N1" s="260"/>
-      <c r="O1" s="260"/>
-      <c r="P1" s="260"/>
+      <c r="A1" s="259" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B1" s="259"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
+      <c r="J1" s="259"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
+      <c r="N1" s="259"/>
+      <c r="O1" s="259"/>
+      <c r="P1" s="259"/>
     </row>
     <row r="3" spans="1:16" ht="45" customHeight="1">
-      <c r="A3" s="224" t="s">
+      <c r="A3" s="223" t="s">
         <v>881</v>
       </c>
-      <c r="B3" s="225" t="s">
+      <c r="B3" s="224" t="s">
         <v>882</v>
       </c>
-      <c r="C3" s="226" t="s">
+      <c r="C3" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="226" t="s">
+      <c r="D3" s="225" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="227" t="s">
+      <c r="E3" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="226" t="s">
+      <c r="F3" s="225" t="s">
         <v>880</v>
       </c>
-      <c r="G3" s="228" t="s">
-        <v>1845</v>
-      </c>
-      <c r="H3" s="226" t="s">
+      <c r="G3" s="227" t="s">
+        <v>1843</v>
+      </c>
+      <c r="H3" s="225" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="228" t="s">
+      <c r="I3" s="227" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="228" t="s">
+      <c r="J3" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="229" t="s">
+      <c r="K3" s="228" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="226" t="s">
+      <c r="L3" s="225" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="226" t="s">
+      <c r="M3" s="225" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="226" t="s">
+      <c r="N3" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="226" t="s">
+      <c r="O3" s="225" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="226" t="s">
+      <c r="P3" s="225" t="s">
         <v>4</v>
       </c>
     </row>
@@ -25921,7 +25897,7 @@
       <c r="I4" s="175">
         <v>6413400</v>
       </c>
-      <c r="J4" s="230">
+      <c r="J4" s="229">
         <v>6413400</v>
       </c>
       <c r="K4" s="177">
@@ -29150,7 +29126,7 @@
         <v>40655</v>
       </c>
       <c r="F71" s="43" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="G71" s="75" t="s">
         <v>1617</v>
@@ -29294,7 +29270,7 @@
         <v>40689</v>
       </c>
       <c r="F74" s="43" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="G74" s="75" t="s">
         <v>1618</v>
@@ -29636,7 +29612,7 @@
         <v>40777</v>
       </c>
       <c r="F81" s="43" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="G81" s="75" t="s">
         <v>1621</v>
@@ -29686,7 +29662,7 @@
         <v>40786</v>
       </c>
       <c r="F82" s="43" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="G82" s="75" t="s">
         <v>1620</v>
@@ -30266,7 +30242,7 @@
         <v>40879</v>
       </c>
       <c r="F94" s="43" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="G94" s="75" t="s">
         <v>1618</v>
@@ -30458,7 +30434,7 @@
         <v>40918</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="G98" s="75" t="s">
         <v>1625</v>
@@ -30554,7 +30530,7 @@
         <v>40924</v>
       </c>
       <c r="F100" s="43" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="G100" s="75" t="s">
         <v>1622</v>
@@ -30794,7 +30770,7 @@
         <v>40956</v>
       </c>
       <c r="F105" s="43" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="G105" s="75" t="s">
         <v>1618</v>
@@ -30842,7 +30818,7 @@
         <v>40961</v>
       </c>
       <c r="F106" s="43" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="G106" s="75" t="s">
         <v>1626</v>
@@ -30988,7 +30964,7 @@
         <v>40976</v>
       </c>
       <c r="F109" s="43" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="G109" s="75" t="s">
         <v>1618</v>
@@ -38085,7 +38061,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="257" spans="1:17" ht="85" customHeight="1">
+    <row r="257" spans="1:16" ht="85" customHeight="1">
       <c r="A257" s="134" t="s">
         <v>50</v>
       </c>
@@ -38133,7 +38109,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="258" spans="1:17" ht="89.75" customHeight="1">
+    <row r="258" spans="1:16" ht="89.75" customHeight="1">
       <c r="A258" s="134" t="s">
         <v>50</v>
       </c>
@@ -38181,7 +38157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="259" spans="1:17" ht="85" customHeight="1">
+    <row r="259" spans="1:16" ht="85" customHeight="1">
       <c r="A259" s="134" t="s">
         <v>50</v>
       </c>
@@ -38229,7 +38205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="260" spans="1:17" ht="85" customHeight="1">
+    <row r="260" spans="1:16" ht="85" customHeight="1">
       <c r="A260" s="134" t="s">
         <v>50</v>
       </c>
@@ -38277,7 +38253,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="261" spans="1:17" ht="74.75" customHeight="1">
+    <row r="261" spans="1:16" ht="74.75" customHeight="1">
       <c r="A261" s="94" t="s">
         <v>421</v>
       </c>
@@ -38302,7 +38278,7 @@
       <c r="H261" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I261" s="253" t="s">
+      <c r="I261" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J261" s="155">
@@ -38325,7 +38301,7 @@
       </c>
       <c r="P261" s="94"/>
     </row>
-    <row r="262" spans="1:17" ht="74.75" customHeight="1">
+    <row r="262" spans="1:16" ht="74.75" customHeight="1">
       <c r="A262" s="94" t="s">
         <v>421</v>
       </c>
@@ -38350,7 +38326,7 @@
       <c r="H262" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I262" s="253" t="s">
+      <c r="I262" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J262" s="155">
@@ -38373,7 +38349,7 @@
       </c>
       <c r="P262" s="94"/>
     </row>
-    <row r="263" spans="1:17" ht="74.75" customHeight="1">
+    <row r="263" spans="1:16" ht="74.75" customHeight="1">
       <c r="A263" s="94" t="s">
         <v>421</v>
       </c>
@@ -38398,7 +38374,7 @@
       <c r="H263" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I263" s="253" t="s">
+      <c r="I263" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J263" s="155">
@@ -38423,7 +38399,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="264" spans="1:17" ht="74.75" customHeight="1">
+    <row r="264" spans="1:16" ht="74.75" customHeight="1">
       <c r="A264" s="91" t="s">
         <v>1096</v>
       </c>
@@ -38448,7 +38424,7 @@
       <c r="H264" s="77" t="s">
         <v>1101</v>
       </c>
-      <c r="I264" s="253" t="s">
+      <c r="I264" s="252" t="s">
         <v>1102</v>
       </c>
       <c r="J264" s="148">
@@ -38473,7 +38449,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="265" spans="1:17" ht="74.75" customHeight="1">
+    <row r="265" spans="1:16" ht="74.75" customHeight="1">
       <c r="A265" s="94" t="s">
         <v>421</v>
       </c>
@@ -38498,7 +38474,7 @@
       <c r="H265" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I265" s="253" t="s">
+      <c r="I265" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J265" s="155">
@@ -38521,7 +38497,7 @@
       </c>
       <c r="P265" s="94"/>
     </row>
-    <row r="266" spans="1:17" ht="73.25" customHeight="1">
+    <row r="266" spans="1:16" ht="73.25" customHeight="1">
       <c r="A266" s="94" t="s">
         <v>421</v>
       </c>
@@ -38546,7 +38522,7 @@
       <c r="H266" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I266" s="253" t="s">
+      <c r="I266" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J266" s="126" t="s">
@@ -38568,11 +38544,8 @@
         <v>1806</v>
       </c>
       <c r="P266" s="94"/>
-      <c r="Q266" s="14" t="s">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="267" spans="1:17" ht="74" customHeight="1">
+    </row>
+    <row r="267" spans="1:16" ht="74" customHeight="1">
       <c r="A267" s="94" t="s">
         <v>421</v>
       </c>
@@ -38597,7 +38570,7 @@
       <c r="H267" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I267" s="253" t="s">
+      <c r="I267" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J267" s="155">
@@ -38620,7 +38593,7 @@
       </c>
       <c r="P267" s="94"/>
     </row>
-    <row r="268" spans="1:17" ht="74" customHeight="1">
+    <row r="268" spans="1:16" ht="74" customHeight="1">
       <c r="A268" s="94" t="s">
         <v>421</v>
       </c>
@@ -38645,7 +38618,7 @@
       <c r="H268" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I268" s="253" t="s">
+      <c r="I268" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J268" s="88">
@@ -38668,7 +38641,7 @@
       </c>
       <c r="P268" s="83"/>
     </row>
-    <row r="269" spans="1:17" ht="74" customHeight="1">
+    <row r="269" spans="1:16" ht="74" customHeight="1">
       <c r="A269" s="94" t="s">
         <v>421</v>
       </c>
@@ -38693,7 +38666,7 @@
       <c r="H269" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I269" s="253" t="s">
+      <c r="I269" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J269" s="155">
@@ -38716,7 +38689,7 @@
       </c>
       <c r="P269" s="94"/>
     </row>
-    <row r="270" spans="1:17" ht="74" customHeight="1">
+    <row r="270" spans="1:16" ht="74" customHeight="1">
       <c r="A270" s="94" t="s">
         <v>421</v>
       </c>
@@ -38741,7 +38714,7 @@
       <c r="H270" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I270" s="253" t="s">
+      <c r="I270" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J270" s="155">
@@ -38764,7 +38737,7 @@
       </c>
       <c r="P270" s="91"/>
     </row>
-    <row r="271" spans="1:17" ht="74" customHeight="1">
+    <row r="271" spans="1:16" ht="74" customHeight="1">
       <c r="A271" s="94" t="s">
         <v>421</v>
       </c>
@@ -38789,7 +38762,7 @@
       <c r="H271" s="77" t="s">
         <v>426</v>
       </c>
-      <c r="I271" s="253" t="s">
+      <c r="I271" s="252" t="s">
         <v>427</v>
       </c>
       <c r="J271" s="155">
@@ -38814,7 +38787,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="272" spans="1:17" ht="116.75" customHeight="1">
+    <row r="272" spans="1:16" ht="116.75" customHeight="1">
       <c r="A272" s="98" t="s">
         <v>1111</v>
       </c>
@@ -39221,13 +39194,13 @@
       <c r="H280" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="I280" s="254" t="s">
+      <c r="I280" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J280" s="156">
         <v>8998500</v>
       </c>
-      <c r="K280" s="255" t="s">
+      <c r="K280" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L280" s="5">
@@ -39269,13 +39242,13 @@
       <c r="H281" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I281" s="254" t="s">
+      <c r="I281" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J281" s="156">
         <v>2080000</v>
       </c>
-      <c r="K281" s="255" t="s">
+      <c r="K281" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L281" s="5">
@@ -39317,13 +39290,13 @@
       <c r="H282" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I282" s="254" t="s">
+      <c r="I282" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J282" s="157">
         <v>1999000</v>
       </c>
-      <c r="K282" s="255" t="s">
+      <c r="K282" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L282" s="5">
@@ -39365,13 +39338,13 @@
       <c r="H283" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I283" s="254" t="s">
+      <c r="I283" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J283" s="156">
         <v>1040000</v>
       </c>
-      <c r="K283" s="255" t="s">
+      <c r="K283" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L283" s="5">
@@ -39413,13 +39386,13 @@
       <c r="H284" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="I284" s="254" t="s">
+      <c r="I284" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J284" s="156">
         <v>2128920</v>
       </c>
-      <c r="K284" s="255" t="s">
+      <c r="K284" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L284" s="5">
@@ -39461,13 +39434,13 @@
       <c r="H285" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I285" s="254" t="s">
+      <c r="I285" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J285" s="156">
         <v>4000000</v>
       </c>
-      <c r="K285" s="255" t="s">
+      <c r="K285" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L285" s="5">
@@ -39509,13 +39482,13 @@
       <c r="H286" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I286" s="254" t="s">
+      <c r="I286" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J286" s="156">
         <v>1758900</v>
       </c>
-      <c r="K286" s="255" t="s">
+      <c r="K286" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L286" s="5">
@@ -39557,13 +39530,13 @@
       <c r="H287" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I287" s="254" t="s">
+      <c r="I287" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J287" s="156">
         <v>22269000</v>
       </c>
-      <c r="K287" s="255" t="s">
+      <c r="K287" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L287" s="5">
@@ -39605,13 +39578,13 @@
       <c r="H288" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I288" s="254" t="s">
+      <c r="I288" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J288" s="156">
         <v>18200000</v>
       </c>
-      <c r="K288" s="255" t="s">
+      <c r="K288" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L288" s="5">
@@ -39653,13 +39626,13 @@
       <c r="H289" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="I289" s="254" t="s">
+      <c r="I289" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J289" s="156">
         <v>8359000</v>
       </c>
-      <c r="K289" s="255" t="s">
+      <c r="K289" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L289" s="5">
@@ -39701,13 +39674,13 @@
       <c r="H290" s="44" t="s">
         <v>517</v>
       </c>
-      <c r="I290" s="254" t="s">
+      <c r="I290" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J290" s="157">
         <v>6500000</v>
       </c>
-      <c r="K290" s="255" t="s">
+      <c r="K290" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L290" s="5">
@@ -39749,13 +39722,13 @@
       <c r="H291" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I291" s="254" t="s">
+      <c r="I291" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J291" s="156">
         <v>9100000</v>
       </c>
-      <c r="K291" s="255" t="s">
+      <c r="K291" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L291" s="5">
@@ -39797,13 +39770,13 @@
       <c r="H292" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I292" s="254" t="s">
+      <c r="I292" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J292" s="156">
         <v>6630000</v>
       </c>
-      <c r="K292" s="255" t="s">
+      <c r="K292" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L292" s="5">
@@ -39845,13 +39818,13 @@
       <c r="H293" s="44" t="s">
         <v>524</v>
       </c>
-      <c r="I293" s="254" t="s">
+      <c r="I293" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J293" s="156">
         <v>6580000</v>
       </c>
-      <c r="K293" s="255" t="s">
+      <c r="K293" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L293" s="5">
@@ -39893,13 +39866,13 @@
       <c r="H294" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I294" s="254" t="s">
+      <c r="I294" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J294" s="156">
         <v>2990000</v>
       </c>
-      <c r="K294" s="255" t="s">
+      <c r="K294" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L294" s="5">
@@ -39941,13 +39914,13 @@
       <c r="H295" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I295" s="254" t="s">
+      <c r="I295" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J295" s="156">
         <v>2992000</v>
       </c>
-      <c r="K295" s="255" t="s">
+      <c r="K295" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L295" s="5">
@@ -39989,13 +39962,13 @@
       <c r="H296" s="44" t="s">
         <v>524</v>
       </c>
-      <c r="I296" s="254" t="s">
+      <c r="I296" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J296" s="156">
         <v>6500000</v>
       </c>
-      <c r="K296" s="255" t="s">
+      <c r="K296" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L296" s="5">
@@ -40037,13 +40010,13 @@
       <c r="H297" s="44" t="s">
         <v>524</v>
       </c>
-      <c r="I297" s="254" t="s">
+      <c r="I297" s="253" t="s">
         <v>493</v>
       </c>
       <c r="J297" s="156">
         <v>15999900</v>
       </c>
-      <c r="K297" s="255" t="s">
+      <c r="K297" s="254" t="s">
         <v>493</v>
       </c>
       <c r="L297" s="5">
@@ -40085,13 +40058,13 @@
       <c r="H298" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I298" s="254" t="s">
+      <c r="I298" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J298" s="156">
         <v>3380000</v>
       </c>
-      <c r="K298" s="255" t="s">
+      <c r="K298" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L298" s="5">
@@ -40133,13 +40106,13 @@
       <c r="H299" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I299" s="254" t="s">
+      <c r="I299" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J299" s="156">
         <v>1690000</v>
       </c>
-      <c r="K299" s="255" t="s">
+      <c r="K299" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L299" s="5">
@@ -40181,13 +40154,13 @@
       <c r="H300" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I300" s="254" t="s">
+      <c r="I300" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J300" s="156">
         <v>5100000</v>
       </c>
-      <c r="K300" s="255" t="s">
+      <c r="K300" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L300" s="5">
@@ -40229,13 +40202,13 @@
       <c r="H301" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I301" s="254" t="s">
+      <c r="I301" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J301" s="156">
         <v>2860000</v>
       </c>
-      <c r="K301" s="255" t="s">
+      <c r="K301" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L301" s="86">
@@ -40277,13 +40250,13 @@
       <c r="H302" s="44" t="s">
         <v>524</v>
       </c>
-      <c r="I302" s="254" t="s">
+      <c r="I302" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J302" s="156">
         <v>61996485</v>
       </c>
-      <c r="K302" s="255" t="s">
+      <c r="K302" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L302" s="86">
@@ -40325,13 +40298,13 @@
       <c r="H303" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I303" s="254" t="s">
+      <c r="I303" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J303" s="156">
         <v>29500000</v>
       </c>
-      <c r="K303" s="255" t="s">
+      <c r="K303" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L303" s="86">
@@ -40373,13 +40346,13 @@
       <c r="H304" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I304" s="254" t="s">
+      <c r="I304" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J304" s="156">
         <v>26999100</v>
       </c>
-      <c r="K304" s="255" t="s">
+      <c r="K304" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L304" s="5">
@@ -40421,13 +40394,13 @@
       <c r="H305" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I305" s="254" t="s">
+      <c r="I305" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J305" s="156">
         <v>22000000</v>
       </c>
-      <c r="K305" s="255" t="s">
+      <c r="K305" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L305" s="5">
@@ -40469,13 +40442,13 @@
       <c r="H306" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="I306" s="254" t="s">
+      <c r="I306" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J306" s="156">
         <v>17225000</v>
       </c>
-      <c r="K306" s="255" t="s">
+      <c r="K306" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L306" s="5">
@@ -40517,13 +40490,13 @@
       <c r="H307" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="I307" s="254" t="s">
+      <c r="I307" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J307" s="156">
         <v>72800000</v>
       </c>
-      <c r="K307" s="255" t="s">
+      <c r="K307" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L307" s="5">
@@ -40565,13 +40538,13 @@
       <c r="H308" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I308" s="254" t="s">
+      <c r="I308" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J308" s="156">
         <v>22100000</v>
       </c>
-      <c r="K308" s="255" t="s">
+      <c r="K308" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L308" s="5">
@@ -40613,13 +40586,13 @@
       <c r="H309" s="44" t="s">
         <v>517</v>
       </c>
-      <c r="I309" s="254" t="s">
+      <c r="I309" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J309" s="156">
         <v>24271000</v>
       </c>
-      <c r="K309" s="255" t="s">
+      <c r="K309" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L309" s="5">
@@ -40661,13 +40634,13 @@
       <c r="H310" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I310" s="254" t="s">
+      <c r="I310" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J310" s="156">
         <v>30940000</v>
       </c>
-      <c r="K310" s="255" t="s">
+      <c r="K310" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L310" s="5">
@@ -40709,13 +40682,13 @@
       <c r="H311" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="I311" s="254" t="s">
+      <c r="I311" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J311" s="156">
         <v>1521360</v>
       </c>
-      <c r="K311" s="255" t="s">
+      <c r="K311" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L311" s="5">
@@ -40757,13 +40730,13 @@
       <c r="H312" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I312" s="254" t="s">
+      <c r="I312" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J312" s="156">
         <v>11999906</v>
       </c>
-      <c r="K312" s="255" t="s">
+      <c r="K312" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L312" s="5">
@@ -40805,13 +40778,13 @@
       <c r="H313" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I313" s="254" t="s">
+      <c r="I313" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J313" s="156">
         <v>26000362</v>
       </c>
-      <c r="K313" s="255" t="s">
+      <c r="K313" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L313" s="5">
@@ -40853,13 +40826,13 @@
       <c r="H314" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I314" s="254" t="s">
+      <c r="I314" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J314" s="157">
         <v>4334000</v>
       </c>
-      <c r="K314" s="255" t="s">
+      <c r="K314" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L314" s="5">
@@ -40901,13 +40874,13 @@
       <c r="H315" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I315" s="254" t="s">
+      <c r="I315" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J315" s="157">
         <v>16900000</v>
       </c>
-      <c r="K315" s="255" t="s">
+      <c r="K315" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L315" s="5">
@@ -40949,13 +40922,13 @@
       <c r="H316" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I316" s="254" t="s">
+      <c r="I316" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J316" s="156">
         <v>28366000</v>
       </c>
-      <c r="K316" s="255" t="s">
+      <c r="K316" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L316" s="5">
@@ -40997,13 +40970,13 @@
       <c r="H317" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I317" s="254" t="s">
+      <c r="I317" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J317" s="156">
         <v>29500000</v>
       </c>
-      <c r="K317" s="255" t="s">
+      <c r="K317" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L317" s="5">
@@ -41045,13 +41018,13 @@
       <c r="H318" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="I318" s="254" t="s">
+      <c r="I318" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J318" s="156">
         <v>4638816</v>
       </c>
-      <c r="K318" s="255" t="s">
+      <c r="K318" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L318" s="5">
@@ -41093,13 +41066,13 @@
       <c r="H319" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I319" s="254" t="s">
+      <c r="I319" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J319" s="156">
         <v>7800000</v>
       </c>
-      <c r="K319" s="255" t="s">
+      <c r="K319" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L319" s="5">
@@ -41141,13 +41114,13 @@
       <c r="H320" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I320" s="254" t="s">
+      <c r="I320" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J320" s="156">
         <v>7709000</v>
       </c>
-      <c r="K320" s="255" t="s">
+      <c r="K320" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L320" s="5">
@@ -41189,13 +41162,13 @@
       <c r="H321" s="44" t="s">
         <v>566</v>
       </c>
-      <c r="I321" s="254" t="s">
+      <c r="I321" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J321" s="156">
         <v>9633792</v>
       </c>
-      <c r="K321" s="255" t="s">
+      <c r="K321" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L321" s="5">
@@ -41237,13 +41210,13 @@
       <c r="H322" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="I322" s="254" t="s">
+      <c r="I322" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J322" s="156">
         <v>17148300</v>
       </c>
-      <c r="K322" s="255" t="s">
+      <c r="K322" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L322" s="5">
@@ -41285,13 +41258,13 @@
       <c r="H323" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="I323" s="254" t="s">
+      <c r="I323" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J323" s="156">
         <v>17951028</v>
       </c>
-      <c r="K323" s="255" t="s">
+      <c r="K323" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L323" s="5">
@@ -41333,13 +41306,13 @@
       <c r="H324" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I324" s="254" t="s">
+      <c r="I324" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J324" s="156">
         <v>2600000</v>
       </c>
-      <c r="K324" s="255" t="s">
+      <c r="K324" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L324" s="5">
@@ -41381,13 +41354,13 @@
       <c r="H325" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I325" s="254" t="s">
+      <c r="I325" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J325" s="156">
         <v>3250000</v>
       </c>
-      <c r="K325" s="255" t="s">
+      <c r="K325" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L325" s="86">
@@ -41429,13 +41402,13 @@
       <c r="H326" s="44" t="s">
         <v>501</v>
       </c>
-      <c r="I326" s="254" t="s">
+      <c r="I326" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J326" s="156">
         <v>8255000</v>
       </c>
-      <c r="K326" s="255" t="s">
+      <c r="K326" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L326" s="86">
@@ -41477,13 +41450,13 @@
       <c r="H327" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="I327" s="254" t="s">
+      <c r="I327" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J327" s="156">
         <v>14902272</v>
       </c>
-      <c r="K327" s="255" t="s">
+      <c r="K327" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L327" s="86">
@@ -41525,13 +41498,13 @@
       <c r="H328" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="I328" s="254" t="s">
+      <c r="I328" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J328" s="156">
         <v>11025000</v>
       </c>
-      <c r="K328" s="255" t="s">
+      <c r="K328" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L328" s="86">
@@ -41573,13 +41546,13 @@
       <c r="H329" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="I329" s="254" t="s">
+      <c r="I329" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J329" s="156">
         <v>11739000</v>
       </c>
-      <c r="K329" s="255" t="s">
+      <c r="K329" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L329" s="86">
@@ -41621,13 +41594,13 @@
       <c r="H330" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="I330" s="254" t="s">
+      <c r="I330" s="253" t="s">
         <v>492</v>
       </c>
       <c r="J330" s="156">
         <v>4956000</v>
       </c>
-      <c r="K330" s="255" t="s">
+      <c r="K330" s="254" t="s">
         <v>492</v>
       </c>
       <c r="L330" s="86">
@@ -41984,7 +41957,7 @@
       <c r="O337" s="96" t="s">
         <v>1806</v>
       </c>
-      <c r="P337" s="231" t="s">
+      <c r="P337" s="230" t="s">
         <v>609</v>
       </c>
     </row>
@@ -42470,7 +42443,7 @@
       <c r="O347" s="96" t="s">
         <v>1806</v>
       </c>
-      <c r="P347" s="232" t="s">
+      <c r="P347" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42520,7 +42493,7 @@
       <c r="O348" s="191">
         <v>1</v>
       </c>
-      <c r="P348" s="232" t="s">
+      <c r="P348" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42570,7 +42543,7 @@
       <c r="O349" s="191">
         <v>1</v>
       </c>
-      <c r="P349" s="232" t="s">
+      <c r="P349" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42620,7 +42593,7 @@
       <c r="O350" s="191">
         <v>3</v>
       </c>
-      <c r="P350" s="232" t="s">
+      <c r="P350" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42670,7 +42643,7 @@
       <c r="O351" s="191">
         <v>3</v>
       </c>
-      <c r="P351" s="232" t="s">
+      <c r="P351" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42720,7 +42693,7 @@
       <c r="O352" s="191">
         <v>1</v>
       </c>
-      <c r="P352" s="232" t="s">
+      <c r="P352" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -42770,7 +42743,7 @@
       <c r="O353" s="191">
         <v>21</v>
       </c>
-      <c r="P353" s="232" t="s">
+      <c r="P353" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42820,7 +42793,7 @@
       <c r="O354" s="191">
         <v>1</v>
       </c>
-      <c r="P354" s="232" t="s">
+      <c r="P354" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42870,7 +42843,7 @@
       <c r="O355" s="191">
         <v>1</v>
       </c>
-      <c r="P355" s="232" t="s">
+      <c r="P355" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -42920,7 +42893,7 @@
       <c r="O356" s="191">
         <v>1</v>
       </c>
-      <c r="P356" s="232" t="s">
+      <c r="P356" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -42970,7 +42943,7 @@
       <c r="O357" s="191">
         <v>1</v>
       </c>
-      <c r="P357" s="232" t="s">
+      <c r="P357" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -43020,7 +42993,7 @@
       <c r="O358" s="191">
         <v>1</v>
       </c>
-      <c r="P358" s="232" t="s">
+      <c r="P358" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43070,7 +43043,7 @@
       <c r="O359" s="191">
         <v>1</v>
       </c>
-      <c r="P359" s="232" t="s">
+      <c r="P359" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -43120,7 +43093,7 @@
       <c r="O360" s="191">
         <v>1</v>
       </c>
-      <c r="P360" s="232" t="s">
+      <c r="P360" s="231" t="s">
         <v>663</v>
       </c>
     </row>
@@ -43170,7 +43143,7 @@
       <c r="O361" s="191">
         <v>9</v>
       </c>
-      <c r="P361" s="232" t="s">
+      <c r="P361" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -43220,7 +43193,7 @@
       <c r="O362" s="191">
         <v>1</v>
       </c>
-      <c r="P362" s="232" t="s">
+      <c r="P362" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43270,7 +43243,7 @@
       <c r="O363" s="191">
         <v>1</v>
       </c>
-      <c r="P363" s="232" t="s">
+      <c r="P363" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43320,7 +43293,7 @@
       <c r="O364" s="191">
         <v>1</v>
       </c>
-      <c r="P364" s="232" t="s">
+      <c r="P364" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -43370,7 +43343,7 @@
       <c r="O365" s="191">
         <v>3</v>
       </c>
-      <c r="P365" s="232" t="s">
+      <c r="P365" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43420,7 +43393,7 @@
       <c r="O366" s="191">
         <v>1</v>
       </c>
-      <c r="P366" s="232" t="s">
+      <c r="P366" s="231" t="s">
         <v>59</v>
       </c>
     </row>
@@ -43470,7 +43443,7 @@
       <c r="O367" s="191">
         <v>1</v>
       </c>
-      <c r="P367" s="232" t="s">
+      <c r="P367" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43520,7 +43493,7 @@
       <c r="O368" s="191">
         <v>1</v>
       </c>
-      <c r="P368" s="232" t="s">
+      <c r="P368" s="231" t="s">
         <v>650</v>
       </c>
     </row>
@@ -43570,7 +43543,7 @@
       <c r="O369" s="191">
         <v>1</v>
       </c>
-      <c r="P369" s="233" t="s">
+      <c r="P369" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43620,7 +43593,7 @@
       <c r="O370" s="191">
         <v>3</v>
       </c>
-      <c r="P370" s="233" t="s">
+      <c r="P370" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43670,7 +43643,7 @@
       <c r="O371" s="191">
         <v>1</v>
       </c>
-      <c r="P371" s="233" t="s">
+      <c r="P371" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43720,7 +43693,7 @@
       <c r="O372" s="191">
         <v>1</v>
       </c>
-      <c r="P372" s="233" t="s">
+      <c r="P372" s="232" t="s">
         <v>663</v>
       </c>
     </row>
@@ -43770,7 +43743,7 @@
       <c r="O373" s="191">
         <v>1</v>
       </c>
-      <c r="P373" s="233" t="s">
+      <c r="P373" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43820,7 +43793,7 @@
       <c r="O374" s="191">
         <v>1</v>
       </c>
-      <c r="P374" s="233" t="s">
+      <c r="P374" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43870,7 +43843,7 @@
       <c r="O375" s="191">
         <v>3</v>
       </c>
-      <c r="P375" s="233" t="s">
+      <c r="P375" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -43968,7 +43941,7 @@
       <c r="O377" s="104">
         <v>1</v>
       </c>
-      <c r="P377" s="233" t="s">
+      <c r="P377" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44066,7 +44039,7 @@
       <c r="O379" s="104">
         <v>1</v>
       </c>
-      <c r="P379" s="233" t="s">
+      <c r="P379" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44214,7 +44187,7 @@
       <c r="O382" s="104">
         <v>1</v>
       </c>
-      <c r="P382" s="233" t="s">
+      <c r="P382" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44264,7 +44237,7 @@
       <c r="O383" s="104">
         <v>1</v>
       </c>
-      <c r="P383" s="233" t="s">
+      <c r="P383" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44410,7 +44383,7 @@
       <c r="O386" s="13">
         <v>1</v>
       </c>
-      <c r="P386" s="233" t="s">
+      <c r="P386" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44556,7 +44529,7 @@
       <c r="O389" s="13">
         <v>1</v>
       </c>
-      <c r="P389" s="233"/>
+      <c r="P389" s="232"/>
     </row>
     <row r="390" spans="1:16" ht="61" customHeight="1">
       <c r="A390" s="193" t="s">
@@ -44604,7 +44577,7 @@
       <c r="O390" s="104">
         <v>1</v>
       </c>
-      <c r="P390" s="233" t="s">
+      <c r="P390" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44654,7 +44627,7 @@
       <c r="O391" s="104">
         <v>1</v>
       </c>
-      <c r="P391" s="233" t="s">
+      <c r="P391" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44704,7 +44677,7 @@
       <c r="O392" s="13">
         <v>1</v>
       </c>
-      <c r="P392" s="233" t="s">
+      <c r="P392" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -44998,7 +44971,7 @@
       <c r="O398" s="104">
         <v>1</v>
       </c>
-      <c r="P398" s="233" t="s">
+      <c r="P398" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -45048,7 +45021,7 @@
       <c r="O399" s="104">
         <v>1</v>
       </c>
-      <c r="P399" s="233" t="s">
+      <c r="P399" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -45098,7 +45071,7 @@
       <c r="O400" s="104">
         <v>1</v>
       </c>
-      <c r="P400" s="233" t="s">
+      <c r="P400" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -45148,7 +45121,7 @@
       <c r="O401" s="13">
         <v>1</v>
       </c>
-      <c r="P401" s="233" t="s">
+      <c r="P401" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -45198,7 +45171,7 @@
       <c r="O402" s="13">
         <v>1</v>
       </c>
-      <c r="P402" s="233" t="s">
+      <c r="P402" s="232" t="s">
         <v>547</v>
       </c>
     </row>
@@ -46840,7 +46813,7 @@
       <c r="O436" s="96" t="s">
         <v>1806</v>
       </c>
-      <c r="P436" s="234" t="s">
+      <c r="P436" s="233" t="s">
         <v>1408</v>
       </c>
     </row>
@@ -48214,7 +48187,7 @@
       </c>
       <c r="P464" s="44"/>
     </row>
-    <row r="465" spans="1:22" ht="100.25" customHeight="1">
+    <row r="465" spans="1:21" ht="100.25" customHeight="1">
       <c r="A465" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48262,7 +48235,7 @@
       </c>
       <c r="P465" s="44"/>
     </row>
-    <row r="466" spans="1:22" ht="100.25" customHeight="1">
+    <row r="466" spans="1:21" ht="100.25" customHeight="1">
       <c r="A466" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48310,7 +48283,7 @@
       </c>
       <c r="P466" s="44"/>
     </row>
-    <row r="467" spans="1:22" s="218" customFormat="1" ht="100.25" customHeight="1">
+    <row r="467" spans="1:21" s="218" customFormat="1" ht="100.25" customHeight="1">
       <c r="A467" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48362,9 +48335,8 @@
       <c r="S467" s="14"/>
       <c r="T467" s="14"/>
       <c r="U467" s="14"/>
-      <c r="V467" s="14"/>
-    </row>
-    <row r="468" spans="1:22" ht="100.25" customHeight="1">
+    </row>
+    <row r="468" spans="1:21" ht="100.25" customHeight="1">
       <c r="A468" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48412,7 +48384,7 @@
       </c>
       <c r="P468" s="44"/>
     </row>
-    <row r="469" spans="1:22" ht="100.25" customHeight="1">
+    <row r="469" spans="1:21" ht="100.25" customHeight="1">
       <c r="A469" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48460,7 +48432,7 @@
       </c>
       <c r="P469" s="44"/>
     </row>
-    <row r="470" spans="1:22" ht="100.25" customHeight="1">
+    <row r="470" spans="1:21" ht="100.25" customHeight="1">
       <c r="A470" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48508,7 +48480,7 @@
       </c>
       <c r="P470" s="44"/>
     </row>
-    <row r="471" spans="1:22" ht="100.25" customHeight="1">
+    <row r="471" spans="1:21" ht="100.25" customHeight="1">
       <c r="A471" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48556,7 +48528,7 @@
       </c>
       <c r="P471" s="44"/>
     </row>
-    <row r="472" spans="1:22" ht="100.25" customHeight="1">
+    <row r="472" spans="1:21" ht="100.25" customHeight="1">
       <c r="A472" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48604,7 +48576,7 @@
       </c>
       <c r="P472" s="44"/>
     </row>
-    <row r="473" spans="1:22" ht="100.25" customHeight="1">
+    <row r="473" spans="1:21" ht="100.25" customHeight="1">
       <c r="A473" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48652,7 +48624,7 @@
       </c>
       <c r="P473" s="44"/>
     </row>
-    <row r="474" spans="1:22" ht="100.25" customHeight="1">
+    <row r="474" spans="1:21" ht="100.25" customHeight="1">
       <c r="A474" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48700,7 +48672,7 @@
       </c>
       <c r="P474" s="44"/>
     </row>
-    <row r="475" spans="1:22" ht="100.25" customHeight="1">
+    <row r="475" spans="1:21" ht="100.25" customHeight="1">
       <c r="A475" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48748,7 +48720,7 @@
       </c>
       <c r="P475" s="44"/>
     </row>
-    <row r="476" spans="1:22" ht="100.25" customHeight="1">
+    <row r="476" spans="1:21" ht="100.25" customHeight="1">
       <c r="A476" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48796,7 +48768,7 @@
       </c>
       <c r="P476" s="44"/>
     </row>
-    <row r="477" spans="1:22" ht="100.25" customHeight="1">
+    <row r="477" spans="1:21" ht="100.25" customHeight="1">
       <c r="A477" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48844,7 +48816,7 @@
       </c>
       <c r="P477" s="44"/>
     </row>
-    <row r="478" spans="1:22" ht="100.25" customHeight="1">
+    <row r="478" spans="1:21" ht="100.25" customHeight="1">
       <c r="A478" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48892,7 +48864,7 @@
       </c>
       <c r="P478" s="44"/>
     </row>
-    <row r="479" spans="1:22" ht="100.25" customHeight="1">
+    <row r="479" spans="1:21" ht="100.25" customHeight="1">
       <c r="A479" s="94" t="s">
         <v>1402</v>
       </c>
@@ -48940,7 +48912,7 @@
       </c>
       <c r="P479" s="44"/>
     </row>
-    <row r="480" spans="1:22" ht="100.25" customHeight="1">
+    <row r="480" spans="1:21" ht="100.25" customHeight="1">
       <c r="A480" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52060,7 +52032,7 @@
       </c>
       <c r="P544" s="82"/>
     </row>
-    <row r="545" spans="1:17" ht="85.75" customHeight="1">
+    <row r="545" spans="1:16" ht="85.75" customHeight="1">
       <c r="A545" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52108,7 +52080,7 @@
       </c>
       <c r="P545" s="82"/>
     </row>
-    <row r="546" spans="1:17" ht="85.75" customHeight="1">
+    <row r="546" spans="1:16" ht="85.75" customHeight="1">
       <c r="A546" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52156,7 +52128,7 @@
       </c>
       <c r="P546" s="82"/>
     </row>
-    <row r="547" spans="1:17" ht="85.75" customHeight="1">
+    <row r="547" spans="1:16" ht="85.75" customHeight="1">
       <c r="A547" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52204,7 +52176,7 @@
       </c>
       <c r="P547" s="82"/>
     </row>
-    <row r="548" spans="1:17" ht="95.75" customHeight="1">
+    <row r="548" spans="1:16" ht="95.75" customHeight="1">
       <c r="A548" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52251,11 +52223,8 @@
         <v>1</v>
       </c>
       <c r="P548" s="103"/>
-      <c r="Q548" s="219" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="549" spans="1:17" ht="95.75" customHeight="1">
+    </row>
+    <row r="549" spans="1:16" ht="95.75" customHeight="1">
       <c r="A549" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52303,7 +52272,7 @@
       </c>
       <c r="P549" s="123"/>
     </row>
-    <row r="550" spans="1:17" ht="72" customHeight="1">
+    <row r="550" spans="1:16" ht="72" customHeight="1">
       <c r="A550" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52351,7 +52320,7 @@
       </c>
       <c r="P550" s="103"/>
     </row>
-    <row r="551" spans="1:17" ht="106.25" customHeight="1">
+    <row r="551" spans="1:16" ht="106.25" customHeight="1">
       <c r="A551" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52399,7 +52368,7 @@
       </c>
       <c r="P551" s="103"/>
     </row>
-    <row r="552" spans="1:17" ht="70.75" customHeight="1">
+    <row r="552" spans="1:16" ht="70.75" customHeight="1">
       <c r="A552" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52445,7 +52414,7 @@
       </c>
       <c r="P552" s="103"/>
     </row>
-    <row r="553" spans="1:17" ht="110.75" customHeight="1">
+    <row r="553" spans="1:16" ht="110.75" customHeight="1">
       <c r="A553" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52491,7 +52460,7 @@
       </c>
       <c r="P553" s="103"/>
     </row>
-    <row r="554" spans="1:17" ht="78.5" customHeight="1">
+    <row r="554" spans="1:16" ht="78.5" customHeight="1">
       <c r="A554" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52541,7 +52510,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="555" spans="1:17" ht="78.5" customHeight="1">
+    <row r="555" spans="1:16" ht="78.5" customHeight="1">
       <c r="A555" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52591,7 +52560,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="556" spans="1:17" ht="78.5" customHeight="1">
+    <row r="556" spans="1:16" ht="78.5" customHeight="1">
       <c r="A556" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52641,7 +52610,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="557" spans="1:17" ht="78.5" customHeight="1">
+    <row r="557" spans="1:16" ht="78.5" customHeight="1">
       <c r="A557" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52689,7 +52658,7 @@
       </c>
       <c r="P557" s="49"/>
     </row>
-    <row r="558" spans="1:17" ht="78.5" customHeight="1">
+    <row r="558" spans="1:16" ht="78.5" customHeight="1">
       <c r="A558" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52739,7 +52708,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="559" spans="1:17" ht="78.5" customHeight="1">
+    <row r="559" spans="1:16" ht="78.5" customHeight="1">
       <c r="A559" s="94" t="s">
         <v>1402</v>
       </c>
@@ -52787,7 +52756,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="560" spans="1:17" ht="86.5" customHeight="1">
+    <row r="560" spans="1:16" ht="86.5" customHeight="1">
       <c r="A560" s="103" t="s">
         <v>1587</v>
       </c>
@@ -53223,7 +53192,7 @@
       <c r="O568" s="83">
         <v>1</v>
       </c>
-      <c r="P568" s="235"/>
+      <c r="P568" s="234"/>
     </row>
     <row r="569" spans="1:16" ht="80.75" customHeight="1">
       <c r="A569" s="94" t="s">
@@ -53346,7 +53315,7 @@
       <c r="H571" s="82" t="s">
         <v>820</v>
       </c>
-      <c r="I571" s="256" t="s">
+      <c r="I571" s="255" t="s">
         <v>821</v>
       </c>
       <c r="J571" s="147">
@@ -53391,7 +53360,7 @@
       <c r="G572" s="76" t="s">
         <v>877</v>
       </c>
-      <c r="H572" s="238" t="s">
+      <c r="H572" s="237" t="s">
         <v>826</v>
       </c>
       <c r="I572" s="166" t="s">
@@ -53400,7 +53369,7 @@
       <c r="J572" s="166">
         <v>1559712</v>
       </c>
-      <c r="K572" s="239" t="s">
+      <c r="K572" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L572" s="91">
@@ -53439,7 +53408,7 @@
       <c r="G573" s="76" t="s">
         <v>1722</v>
       </c>
-      <c r="H573" s="238" t="s">
+      <c r="H573" s="237" t="s">
         <v>832</v>
       </c>
       <c r="I573" s="153" t="s">
@@ -53448,7 +53417,7 @@
       <c r="J573" s="166">
         <v>1228500</v>
       </c>
-      <c r="K573" s="239" t="s">
+      <c r="K573" s="238" t="s">
         <v>1806</v>
       </c>
       <c r="L573" s="91">
@@ -53487,7 +53456,7 @@
       <c r="G574" s="76" t="s">
         <v>1699</v>
       </c>
-      <c r="H574" s="238" t="s">
+      <c r="H574" s="237" t="s">
         <v>826</v>
       </c>
       <c r="I574" s="153" t="s">
@@ -53496,7 +53465,7 @@
       <c r="J574" s="166">
         <v>2773050</v>
       </c>
-      <c r="K574" s="239" t="s">
+      <c r="K574" s="238" t="s">
         <v>1806</v>
       </c>
       <c r="L574" s="91">
@@ -53535,7 +53504,7 @@
       <c r="G575" s="76" t="s">
         <v>1722</v>
       </c>
-      <c r="H575" s="238" t="s">
+      <c r="H575" s="237" t="s">
         <v>826</v>
       </c>
       <c r="I575" s="153" t="s">
@@ -53544,7 +53513,7 @@
       <c r="J575" s="166">
         <v>15340500</v>
       </c>
-      <c r="K575" s="239" t="s">
+      <c r="K575" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L575" s="91">
@@ -53583,7 +53552,7 @@
       <c r="G576" s="76" t="s">
         <v>1699</v>
       </c>
-      <c r="H576" s="238" t="s">
+      <c r="H576" s="237" t="s">
         <v>826</v>
       </c>
       <c r="I576" s="153" t="s">
@@ -53592,7 +53561,7 @@
       <c r="J576" s="166">
         <v>1860600</v>
       </c>
-      <c r="K576" s="239" t="s">
+      <c r="K576" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L576" s="91">
@@ -53637,10 +53606,10 @@
       <c r="I577" s="153" t="s">
         <v>843</v>
       </c>
-      <c r="J577" s="240">
+      <c r="J577" s="239">
         <v>2436000</v>
       </c>
-      <c r="K577" s="239" t="s">
+      <c r="K577" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L577" s="79" t="s">
@@ -53685,10 +53654,10 @@
       <c r="I578" s="153" t="s">
         <v>843</v>
       </c>
-      <c r="J578" s="240">
+      <c r="J578" s="239">
         <v>2942100</v>
       </c>
-      <c r="K578" s="239" t="s">
+      <c r="K578" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L578" s="79" t="s">
@@ -53730,13 +53699,13 @@
       <c r="H579" s="78" t="s">
         <v>888</v>
       </c>
-      <c r="I579" s="257" t="s">
+      <c r="I579" s="256" t="s">
         <v>889</v>
       </c>
       <c r="J579" s="22" t="s">
         <v>890</v>
       </c>
-      <c r="K579" s="239" t="s">
+      <c r="K579" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L579" s="23" t="s">
@@ -53828,7 +53797,7 @@
       <c r="H581" s="78" t="s">
         <v>902</v>
       </c>
-      <c r="I581" s="258" t="s">
+      <c r="I581" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J581" s="22">
@@ -53878,7 +53847,7 @@
       <c r="H582" s="78" t="s">
         <v>907</v>
       </c>
-      <c r="I582" s="258" t="s">
+      <c r="I582" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J582" s="22">
@@ -53928,7 +53897,7 @@
       <c r="H583" s="78" t="s">
         <v>911</v>
       </c>
-      <c r="I583" s="258" t="s">
+      <c r="I583" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J583" s="22">
@@ -53978,7 +53947,7 @@
       <c r="H584" s="78" t="s">
         <v>911</v>
       </c>
-      <c r="I584" s="258" t="s">
+      <c r="I584" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J584" s="22">
@@ -54028,7 +53997,7 @@
       <c r="H585" s="78" t="s">
         <v>916</v>
       </c>
-      <c r="I585" s="258" t="s">
+      <c r="I585" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J585" s="22">
@@ -54078,7 +54047,7 @@
       <c r="H586" s="78" t="s">
         <v>921</v>
       </c>
-      <c r="I586" s="258" t="s">
+      <c r="I586" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J586" s="22">
@@ -54128,7 +54097,7 @@
       <c r="H587" s="78" t="s">
         <v>925</v>
       </c>
-      <c r="I587" s="258" t="s">
+      <c r="I587" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J587" s="22">
@@ -54178,7 +54147,7 @@
       <c r="H588" s="78" t="s">
         <v>925</v>
       </c>
-      <c r="I588" s="258" t="s">
+      <c r="I588" s="257" t="s">
         <v>903</v>
       </c>
       <c r="J588" s="22">
@@ -54228,13 +54197,13 @@
       <c r="H589" s="78" t="s">
         <v>930</v>
       </c>
-      <c r="I589" s="238" t="s">
+      <c r="I589" s="237" t="s">
         <v>931</v>
       </c>
       <c r="J589" s="22">
         <v>46944612</v>
       </c>
-      <c r="K589" s="239" t="s">
+      <c r="K589" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L589" s="78">
@@ -54278,13 +54247,13 @@
       <c r="H590" s="78" t="s">
         <v>934</v>
       </c>
-      <c r="I590" s="238" t="s">
+      <c r="I590" s="237" t="s">
         <v>931</v>
       </c>
       <c r="J590" s="22">
         <v>1130785</v>
       </c>
-      <c r="K590" s="239" t="s">
+      <c r="K590" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L590" s="78">
@@ -54328,13 +54297,13 @@
       <c r="H591" s="78" t="s">
         <v>939</v>
       </c>
-      <c r="I591" s="238" t="s">
+      <c r="I591" s="237" t="s">
         <v>931</v>
       </c>
       <c r="J591" s="22">
         <v>2162000</v>
       </c>
-      <c r="K591" s="239" t="s">
+      <c r="K591" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L591" s="78">
@@ -54401,7 +54370,7 @@
       </c>
       <c r="P592" s="9"/>
     </row>
-    <row r="593" spans="1:22" ht="80.75" customHeight="1">
+    <row r="593" spans="1:21" ht="80.75" customHeight="1">
       <c r="A593" s="9" t="s">
         <v>883</v>
       </c>
@@ -54449,7 +54418,7 @@
       </c>
       <c r="P593" s="9"/>
     </row>
-    <row r="594" spans="1:22" ht="80.75" customHeight="1">
+    <row r="594" spans="1:21" ht="80.75" customHeight="1">
       <c r="A594" s="9" t="s">
         <v>883</v>
       </c>
@@ -54466,7 +54435,7 @@
         <v>40634</v>
       </c>
       <c r="F594" s="21" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="G594" s="78" t="s">
         <v>1749</v>
@@ -54497,7 +54466,7 @@
       </c>
       <c r="P594" s="9"/>
     </row>
-    <row r="595" spans="1:22" ht="65">
+    <row r="595" spans="1:21" ht="65">
       <c r="A595" s="9" t="s">
         <v>883</v>
       </c>
@@ -54522,13 +54491,13 @@
       <c r="H595" s="78" t="s">
         <v>953</v>
       </c>
-      <c r="I595" s="259" t="s">
+      <c r="I595" s="258" t="s">
         <v>1094</v>
       </c>
       <c r="J595" s="166">
         <v>11634000</v>
       </c>
-      <c r="K595" s="239" t="s">
+      <c r="K595" s="238" t="s">
         <v>1810</v>
       </c>
       <c r="L595" s="9">
@@ -54547,7 +54516,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="596" spans="1:22" ht="95" customHeight="1">
+    <row r="596" spans="1:21" ht="95" customHeight="1">
       <c r="A596" s="98" t="s">
         <v>1071</v>
       </c>
@@ -54572,10 +54541,10 @@
       <c r="H596" s="78" t="s">
         <v>1075</v>
       </c>
-      <c r="I596" s="259" t="s">
+      <c r="I596" s="258" t="s">
         <v>1812</v>
       </c>
-      <c r="J596" s="240">
+      <c r="J596" s="239">
         <v>4993800</v>
       </c>
       <c r="K596" s="112" t="s">
@@ -54599,9 +54568,8 @@
       <c r="S596" s="218"/>
       <c r="T596" s="218"/>
       <c r="U596" s="218"/>
-      <c r="V596" s="218"/>
-    </row>
-    <row r="597" spans="1:22" ht="112" customHeight="1">
+    </row>
+    <row r="597" spans="1:21" ht="112" customHeight="1">
       <c r="A597" s="98" t="s">
         <v>1071</v>
       </c>
@@ -54626,10 +54594,10 @@
       <c r="H597" s="78" t="s">
         <v>1082</v>
       </c>
-      <c r="I597" s="259" t="s">
+      <c r="I597" s="258" t="s">
         <v>1812</v>
       </c>
-      <c r="J597" s="240">
+      <c r="J597" s="239">
         <v>3461850</v>
       </c>
       <c r="K597" s="112" t="s">
@@ -54649,7 +54617,7 @@
       </c>
       <c r="P597" s="91"/>
     </row>
-    <row r="598" spans="1:22" ht="83.75" customHeight="1">
+    <row r="598" spans="1:21" ht="83.75" customHeight="1">
       <c r="A598" s="98" t="s">
         <v>1071</v>
       </c>
@@ -54674,10 +54642,10 @@
       <c r="H598" s="78" t="s">
         <v>1089</v>
       </c>
-      <c r="I598" s="259" t="s">
+      <c r="I598" s="258" t="s">
         <v>1812</v>
       </c>
-      <c r="J598" s="240">
+      <c r="J598" s="239">
         <v>5999800</v>
       </c>
       <c r="K598" s="112" t="s">
@@ -54697,7 +54665,7 @@
       </c>
       <c r="P598" s="91"/>
     </row>
-    <row r="599" spans="1:22" ht="102.75" customHeight="1">
+    <row r="599" spans="1:21" ht="102.75" customHeight="1">
       <c r="A599" s="9" t="s">
         <v>883</v>
       </c>
@@ -54747,7 +54715,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="600" spans="1:22" ht="102.75" customHeight="1">
+    <row r="600" spans="1:21" ht="102.75" customHeight="1">
       <c r="A600" s="9" t="s">
         <v>883</v>
       </c>
@@ -54797,7 +54765,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="601" spans="1:22" ht="102.75" customHeight="1">
+    <row r="601" spans="1:21" ht="102.75" customHeight="1">
       <c r="A601" s="9" t="s">
         <v>883</v>
       </c>
@@ -54847,7 +54815,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="602" spans="1:22" ht="85" customHeight="1">
+    <row r="602" spans="1:21" ht="85" customHeight="1">
       <c r="A602" s="9" t="s">
         <v>883</v>
       </c>
@@ -54872,7 +54840,7 @@
       <c r="H602" s="78" t="s">
         <v>970</v>
       </c>
-      <c r="I602" s="258" t="s">
+      <c r="I602" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J602" s="167">
@@ -54897,7 +54865,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="603" spans="1:22" ht="85" customHeight="1">
+    <row r="603" spans="1:21" ht="85" customHeight="1">
       <c r="A603" s="9" t="s">
         <v>883</v>
       </c>
@@ -54922,7 +54890,7 @@
       <c r="H603" s="78" t="s">
         <v>976</v>
       </c>
-      <c r="I603" s="258" t="s">
+      <c r="I603" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J603" s="168">
@@ -54947,7 +54915,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="604" spans="1:22" ht="85" customHeight="1">
+    <row r="604" spans="1:21" ht="85" customHeight="1">
       <c r="A604" s="9" t="s">
         <v>883</v>
       </c>
@@ -54972,7 +54940,7 @@
       <c r="H604" s="78" t="s">
         <v>976</v>
       </c>
-      <c r="I604" s="258" t="s">
+      <c r="I604" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J604" s="168">
@@ -54997,7 +54965,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="605" spans="1:22" ht="85" customHeight="1">
+    <row r="605" spans="1:21" ht="85" customHeight="1">
       <c r="A605" s="9" t="s">
         <v>883</v>
       </c>
@@ -55022,7 +54990,7 @@
       <c r="H605" s="78" t="s">
         <v>976</v>
       </c>
-      <c r="I605" s="258" t="s">
+      <c r="I605" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J605" s="168">
@@ -55047,7 +55015,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="606" spans="1:22" ht="85" customHeight="1">
+    <row r="606" spans="1:21" ht="85" customHeight="1">
       <c r="A606" s="9" t="s">
         <v>883</v>
       </c>
@@ -55072,7 +55040,7 @@
       <c r="H606" s="78" t="s">
         <v>983</v>
       </c>
-      <c r="I606" s="258" t="s">
+      <c r="I606" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J606" s="167">
@@ -55097,7 +55065,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="607" spans="1:22" ht="85" customHeight="1">
+    <row r="607" spans="1:21" ht="85" customHeight="1">
       <c r="A607" s="9" t="s">
         <v>883</v>
       </c>
@@ -55122,7 +55090,7 @@
       <c r="H607" s="78" t="s">
         <v>983</v>
       </c>
-      <c r="I607" s="258" t="s">
+      <c r="I607" s="257" t="s">
         <v>971</v>
       </c>
       <c r="J607" s="167">
@@ -55147,7 +55115,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="608" spans="1:22" ht="89.25" customHeight="1">
+    <row r="608" spans="1:21" ht="89.25" customHeight="1">
       <c r="A608" s="9" t="s">
         <v>883</v>
       </c>
@@ -56305,7 +56273,7 @@
         <v>1160</v>
       </c>
       <c r="C631" s="78" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="D631" s="78" t="s">
         <v>1347</v>
@@ -56372,13 +56340,13 @@
       <c r="H632" s="78" t="s">
         <v>1349</v>
       </c>
-      <c r="I632" s="240">
+      <c r="I632" s="239">
         <v>1050000</v>
       </c>
-      <c r="J632" s="240">
+      <c r="J632" s="239">
         <v>1050000</v>
       </c>
-      <c r="K632" s="241">
+      <c r="K632" s="240">
         <v>1</v>
       </c>
       <c r="L632" s="23" t="s">
@@ -56426,7 +56394,7 @@
       <c r="J633" s="137">
         <v>24515652</v>
       </c>
-      <c r="K633" s="242">
+      <c r="K633" s="241">
         <f>J633/I633</f>
         <v>0.99712389367033316</v>
       </c>
@@ -56646,7 +56614,7 @@
       <c r="C638" s="78" t="s">
         <v>1175</v>
       </c>
-      <c r="D638" s="238" t="s">
+      <c r="D638" s="237" t="s">
         <v>1182</v>
       </c>
       <c r="E638" s="85">
@@ -56709,10 +56677,10 @@
       <c r="H639" s="80" t="s">
         <v>1355</v>
       </c>
-      <c r="I639" s="243" t="s">
+      <c r="I639" s="242" t="s">
         <v>904</v>
       </c>
-      <c r="J639" s="243" t="s">
+      <c r="J639" s="242" t="s">
         <v>1187</v>
       </c>
       <c r="K639" s="112" t="s">
@@ -56759,7 +56727,7 @@
       <c r="H640" s="80" t="s">
         <v>1359</v>
       </c>
-      <c r="I640" s="243" t="s">
+      <c r="I640" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J640" s="137">
@@ -56807,7 +56775,7 @@
       <c r="H641" s="80" t="s">
         <v>1359</v>
       </c>
-      <c r="I641" s="243" t="s">
+      <c r="I641" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J641" s="137">
@@ -56855,7 +56823,7 @@
       <c r="H642" s="80" t="s">
         <v>1359</v>
       </c>
-      <c r="I642" s="243" t="s">
+      <c r="I642" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J642" s="137">
@@ -56903,7 +56871,7 @@
       <c r="H643" s="80" t="s">
         <v>1196</v>
       </c>
-      <c r="I643" s="243" t="s">
+      <c r="I643" s="242" t="s">
         <v>1361</v>
       </c>
       <c r="J643" s="137">
@@ -58105,10 +58073,10 @@
       <c r="H668" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I668" s="243" t="s">
+      <c r="I668" s="242" t="s">
         <v>904</v>
       </c>
-      <c r="J668" s="244">
+      <c r="J668" s="243">
         <v>18270000</v>
       </c>
       <c r="K668" s="112" t="s">
@@ -58144,7 +58112,7 @@
       <c r="E669" s="50">
         <v>40634</v>
       </c>
-      <c r="F669" s="245" t="s">
+      <c r="F669" s="244" t="s">
         <v>1229</v>
       </c>
       <c r="G669" s="78" t="s">
@@ -58153,10 +58121,10 @@
       <c r="H669" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I669" s="243" t="s">
+      <c r="I669" s="242" t="s">
         <v>904</v>
       </c>
-      <c r="J669" s="244">
+      <c r="J669" s="243">
         <v>12999000</v>
       </c>
       <c r="K669" s="112" t="s">
@@ -58201,7 +58169,7 @@
       <c r="H670" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I670" s="243" t="s">
+      <c r="I670" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J670" s="171">
@@ -58249,7 +58217,7 @@
       <c r="H671" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I671" s="243" t="s">
+      <c r="I671" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J671" s="171">
@@ -58297,7 +58265,7 @@
       <c r="H672" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I672" s="243" t="s">
+      <c r="I672" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J672" s="171">
@@ -58345,7 +58313,7 @@
       <c r="H673" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I673" s="243" t="s">
+      <c r="I673" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J673" s="171">
@@ -58384,7 +58352,7 @@
       <c r="E674" s="50">
         <v>40773</v>
       </c>
-      <c r="F674" s="245" t="s">
+      <c r="F674" s="244" t="s">
         <v>1229</v>
       </c>
       <c r="G674" s="78" t="s">
@@ -58393,7 +58361,7 @@
       <c r="H674" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I674" s="243" t="s">
+      <c r="I674" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J674" s="171">
@@ -58432,7 +58400,7 @@
       <c r="E675" s="50">
         <v>40844</v>
       </c>
-      <c r="F675" s="245" t="s">
+      <c r="F675" s="244" t="s">
         <v>1373</v>
       </c>
       <c r="G675" s="78" t="s">
@@ -58441,7 +58409,7 @@
       <c r="H675" s="51" t="s">
         <v>1362</v>
       </c>
-      <c r="I675" s="243" t="s">
+      <c r="I675" s="242" t="s">
         <v>904</v>
       </c>
       <c r="J675" s="171">
@@ -59254,7 +59222,7 @@
       <c r="G692" s="78" t="s">
         <v>1780</v>
       </c>
-      <c r="H692" s="245" t="s">
+      <c r="H692" s="244" t="s">
         <v>1252</v>
       </c>
       <c r="I692" s="148">
@@ -59277,7 +59245,7 @@
       </c>
       <c r="O692" s="79"/>
       <c r="P692" s="23" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="693" spans="1:16" ht="144.5" customHeight="1">
@@ -59314,7 +59282,7 @@
       <c r="K693" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L693" s="246" t="s">
+      <c r="L693" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M693" s="79" t="s">
@@ -59362,7 +59330,7 @@
       <c r="K694" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L694" s="246" t="s">
+      <c r="L694" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M694" s="79" t="s">
@@ -59410,7 +59378,7 @@
       <c r="K695" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L695" s="246" t="s">
+      <c r="L695" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M695" s="79" t="s">
@@ -59458,7 +59426,7 @@
       <c r="K696" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L696" s="246" t="s">
+      <c r="L696" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M696" s="79" t="s">
@@ -59506,7 +59474,7 @@
       <c r="K697" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L697" s="246" t="s">
+      <c r="L697" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M697" s="90" t="s">
@@ -59556,7 +59524,7 @@
       <c r="K698" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L698" s="246" t="s">
+      <c r="L698" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M698" s="90" t="s">
@@ -59606,7 +59574,7 @@
       <c r="K699" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L699" s="246" t="s">
+      <c r="L699" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M699" s="90" t="s">
@@ -59656,7 +59624,7 @@
       <c r="K700" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L700" s="246" t="s">
+      <c r="L700" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M700" s="90" t="s">
@@ -59689,7 +59657,7 @@
         <v>40634</v>
       </c>
       <c r="F701" s="80" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="G701" s="78" t="s">
         <v>1786</v>
@@ -59706,7 +59674,7 @@
       <c r="K701" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L701" s="246" t="s">
+      <c r="L701" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M701" s="90" t="s">
@@ -59756,7 +59724,7 @@
       <c r="K702" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L702" s="246" t="s">
+      <c r="L702" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M702" s="90" t="s">
@@ -59806,7 +59774,7 @@
       <c r="K703" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L703" s="246" t="s">
+      <c r="L703" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M703" s="90" t="s">
@@ -59856,7 +59824,7 @@
       <c r="K704" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L704" s="246" t="s">
+      <c r="L704" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M704" s="90" t="s">
@@ -59906,7 +59874,7 @@
       <c r="K705" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L705" s="246" t="s">
+      <c r="L705" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M705" s="90" t="s">
@@ -59956,7 +59924,7 @@
       <c r="K706" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L706" s="246" t="s">
+      <c r="L706" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M706" s="90" t="s">
@@ -60006,7 +59974,7 @@
       <c r="K707" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L707" s="246" t="s">
+      <c r="L707" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M707" s="90" t="s">
@@ -60056,7 +60024,7 @@
       <c r="K708" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L708" s="246" t="s">
+      <c r="L708" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M708" s="90" t="s">
@@ -60106,7 +60074,7 @@
       <c r="K709" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L709" s="246" t="s">
+      <c r="L709" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M709" s="90" t="s">
@@ -60156,7 +60124,7 @@
       <c r="K710" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L710" s="246" t="s">
+      <c r="L710" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M710" s="90" t="s">
@@ -60189,7 +60157,7 @@
         <v>40634</v>
       </c>
       <c r="F711" s="51" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="G711" s="78" t="s">
         <v>1796</v>
@@ -60206,7 +60174,7 @@
       <c r="K711" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L711" s="246" t="s">
+      <c r="L711" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M711" s="90" t="s">
@@ -60256,7 +60224,7 @@
       <c r="K712" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L712" s="246" t="s">
+      <c r="L712" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M712" s="90" t="s">
@@ -60306,7 +60274,7 @@
       <c r="K713" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L713" s="246" t="s">
+      <c r="L713" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M713" s="90" t="s">
@@ -60356,7 +60324,7 @@
       <c r="K714" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L714" s="246" t="s">
+      <c r="L714" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M714" s="90" t="s">
@@ -60406,7 +60374,7 @@
       <c r="K715" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L715" s="246" t="s">
+      <c r="L715" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M715" s="90" t="s">
@@ -60456,7 +60424,7 @@
       <c r="K716" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L716" s="246" t="s">
+      <c r="L716" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M716" s="90" t="s">
@@ -60707,7 +60675,7 @@
         <v>2</v>
       </c>
       <c r="M721" s="23" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="N721" s="23" t="s">
         <v>49</v>
@@ -60756,7 +60724,7 @@
         <v>2</v>
       </c>
       <c r="M722" s="23" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="N722" s="23" t="s">
         <v>49</v>
@@ -60846,10 +60814,10 @@
       <c r="J724" s="166">
         <v>6720000</v>
       </c>
-      <c r="K724" s="241">
+      <c r="K724" s="240">
         <v>0.99419999999999997</v>
       </c>
-      <c r="L724" s="246" t="s">
+      <c r="L724" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M724" s="79" t="s">
@@ -60897,7 +60865,7 @@
       <c r="K725" s="122">
         <v>1</v>
       </c>
-      <c r="L725" s="246" t="s">
+      <c r="L725" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M725" s="79" t="s">
@@ -60923,7 +60891,7 @@
       <c r="C726" s="62" t="s">
         <v>1336</v>
       </c>
-      <c r="D726" s="238" t="s">
+      <c r="D726" s="237" t="s">
         <v>1337</v>
       </c>
       <c r="E726" s="61">
@@ -60947,7 +60915,7 @@
       <c r="K726" s="120">
         <v>1</v>
       </c>
-      <c r="L726" s="246" t="s">
+      <c r="L726" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M726" s="79" t="s">
@@ -60973,7 +60941,7 @@
       <c r="C727" s="24" t="s">
         <v>1331</v>
       </c>
-      <c r="D727" s="238" t="s">
+      <c r="D727" s="237" t="s">
         <v>1340</v>
       </c>
       <c r="E727" s="64">
@@ -60997,7 +60965,7 @@
       <c r="K727" s="122">
         <v>1</v>
       </c>
-      <c r="L727" s="246" t="s">
+      <c r="L727" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M727" s="79" t="s">
@@ -61023,7 +60991,7 @@
       <c r="C728" s="24" t="s">
         <v>1398</v>
       </c>
-      <c r="D728" s="238" t="s">
+      <c r="D728" s="237" t="s">
         <v>1344</v>
       </c>
       <c r="E728" s="85">
@@ -61047,7 +61015,7 @@
       <c r="K728" s="122">
         <v>1</v>
       </c>
-      <c r="L728" s="246" t="s">
+      <c r="L728" s="245" t="s">
         <v>751</v>
       </c>
       <c r="M728" s="79" t="s">
@@ -61073,7 +61041,7 @@
       <c r="C729" s="62" t="s">
         <v>1336</v>
       </c>
-      <c r="D729" s="238" t="s">
+      <c r="D729" s="237" t="s">
         <v>1337</v>
       </c>
       <c r="E729" s="61">
@@ -61097,7 +61065,7 @@
       <c r="K729" s="120">
         <v>1</v>
       </c>
-      <c r="L729" s="247" t="s">
+      <c r="L729" s="246" t="s">
         <v>751</v>
       </c>
       <c r="M729" s="79" t="s">
@@ -61114,10 +61082,10 @@
       </c>
     </row>
     <row r="730" spans="1:16" ht="200.25" customHeight="1">
-      <c r="A730" s="248" t="s">
+      <c r="A730" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B730" s="249" t="s">
+      <c r="B730" s="248" t="s">
         <v>1126</v>
       </c>
       <c r="C730" s="78" t="s">
@@ -61138,34 +61106,34 @@
       <c r="H730" s="71" t="s">
         <v>1130</v>
       </c>
-      <c r="I730" s="250" t="s">
+      <c r="I730" s="249" t="s">
         <v>1131</v>
       </c>
-      <c r="J730" s="251">
+      <c r="J730" s="250">
         <v>2000000</v>
       </c>
       <c r="K730" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L730" s="248">
+      <c r="L730" s="247">
         <v>0</v>
       </c>
-      <c r="M730" s="252" t="s">
+      <c r="M730" s="251" t="s">
         <v>458</v>
       </c>
-      <c r="N730" s="252" t="s">
+      <c r="N730" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="O730" s="252">
+      <c r="O730" s="251">
         <v>5</v>
       </c>
-      <c r="P730" s="248"/>
+      <c r="P730" s="247"/>
     </row>
     <row r="731" spans="1:16" ht="199.75" customHeight="1">
-      <c r="A731" s="248" t="s">
+      <c r="A731" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B731" s="249" t="s">
+      <c r="B731" s="248" t="s">
         <v>1126</v>
       </c>
       <c r="C731" s="78" t="s">
@@ -61186,34 +61154,34 @@
       <c r="H731" s="71" t="s">
         <v>1134</v>
       </c>
-      <c r="I731" s="250" t="s">
+      <c r="I731" s="249" t="s">
         <v>1135</v>
       </c>
-      <c r="J731" s="251">
+      <c r="J731" s="250">
         <v>1750017</v>
       </c>
       <c r="K731" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L731" s="248">
+      <c r="L731" s="247">
         <v>0</v>
       </c>
-      <c r="M731" s="252" t="s">
+      <c r="M731" s="251" t="s">
         <v>48</v>
       </c>
-      <c r="N731" s="252" t="s">
+      <c r="N731" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="O731" s="252">
+      <c r="O731" s="251">
         <v>2</v>
       </c>
-      <c r="P731" s="248"/>
+      <c r="P731" s="247"/>
     </row>
     <row r="732" spans="1:16" ht="211.75" customHeight="1">
-      <c r="A732" s="248" t="s">
+      <c r="A732" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B732" s="249" t="s">
+      <c r="B732" s="248" t="s">
         <v>1126</v>
       </c>
       <c r="C732" s="78" t="s">
@@ -61234,34 +61202,34 @@
       <c r="H732" s="78" t="s">
         <v>1139</v>
       </c>
-      <c r="I732" s="250" t="s">
+      <c r="I732" s="249" t="s">
         <v>1135</v>
       </c>
-      <c r="J732" s="251">
+      <c r="J732" s="250">
         <v>7807629</v>
       </c>
       <c r="K732" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L732" s="248">
+      <c r="L732" s="247">
         <v>0</v>
       </c>
-      <c r="M732" s="252" t="s">
+      <c r="M732" s="251" t="s">
         <v>591</v>
       </c>
-      <c r="N732" s="252" t="s">
+      <c r="N732" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="O732" s="252">
+      <c r="O732" s="251">
         <v>3</v>
       </c>
-      <c r="P732" s="248"/>
+      <c r="P732" s="247"/>
     </row>
     <row r="733" spans="1:16" ht="203.75" customHeight="1">
-      <c r="A733" s="248" t="s">
+      <c r="A733" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B733" s="249" t="s">
+      <c r="B733" s="248" t="s">
         <v>1126</v>
       </c>
       <c r="C733" s="78" t="s">
@@ -61282,34 +61250,34 @@
       <c r="H733" s="78" t="s">
         <v>1141</v>
       </c>
-      <c r="I733" s="250" t="s">
+      <c r="I733" s="249" t="s">
         <v>1135</v>
       </c>
-      <c r="J733" s="251">
+      <c r="J733" s="250">
         <v>1970357</v>
       </c>
       <c r="K733" s="112" t="s">
         <v>1809</v>
       </c>
-      <c r="L733" s="248">
+      <c r="L733" s="247">
         <v>0</v>
       </c>
-      <c r="M733" s="252" t="s">
+      <c r="M733" s="251" t="s">
         <v>591</v>
       </c>
-      <c r="N733" s="252" t="s">
+      <c r="N733" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="O733" s="252">
+      <c r="O733" s="251">
         <v>5</v>
       </c>
-      <c r="P733" s="248"/>
+      <c r="P733" s="247"/>
     </row>
     <row r="734" spans="1:16" ht="176.75" customHeight="1">
-      <c r="A734" s="248" t="s">
+      <c r="A734" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B734" s="249" t="s">
+      <c r="B734" s="248" t="s">
         <v>1147</v>
       </c>
       <c r="C734" s="80" t="s">
@@ -61351,13 +61319,13 @@
       <c r="O734" s="90" t="s">
         <v>1806</v>
       </c>
-      <c r="P734" s="248"/>
+      <c r="P734" s="247"/>
     </row>
     <row r="735" spans="1:16" ht="189.25" customHeight="1">
-      <c r="A735" s="248" t="s">
+      <c r="A735" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B735" s="249" t="s">
+      <c r="B735" s="248" t="s">
         <v>1147</v>
       </c>
       <c r="C735" s="80" t="s">
@@ -61399,16 +61367,16 @@
       <c r="O735" s="90" t="s">
         <v>1806</v>
       </c>
-      <c r="P735" s="248"/>
+      <c r="P735" s="247"/>
     </row>
     <row r="736" spans="1:16" ht="153.25" customHeight="1">
-      <c r="A736" s="248" t="s">
+      <c r="A736" s="247" t="s">
         <v>1125</v>
       </c>
-      <c r="B736" s="249" t="s">
+      <c r="B736" s="248" t="s">
         <v>1147</v>
       </c>
-      <c r="C736" s="236" t="s">
+      <c r="C736" s="235" t="s">
         <v>1152</v>
       </c>
       <c r="D736" s="80" t="s">
@@ -61447,328 +61415,328 @@
       <c r="O736" s="90" t="s">
         <v>1807</v>
       </c>
-      <c r="P736" s="248"/>
+      <c r="P736" s="247"/>
     </row>
     <row r="737" spans="1:15" ht="18" customHeight="1">
-      <c r="A737" s="237" t="s">
-        <v>1846</v>
-      </c>
-      <c r="C737" s="223"/>
+      <c r="A737" s="236" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C737" s="222"/>
       <c r="D737" s="40"/>
-      <c r="E737" s="220"/>
+      <c r="E737" s="219"/>
       <c r="F737" s="40"/>
       <c r="G737" s="40"/>
       <c r="H737" s="40"/>
-      <c r="I737" s="221"/>
-      <c r="J737" s="221"/>
-      <c r="K737" s="222"/>
+      <c r="I737" s="220"/>
+      <c r="J737" s="220"/>
+      <c r="K737" s="221"/>
       <c r="L737" s="40"/>
       <c r="M737" s="40"/>
       <c r="N737" s="40"/>
       <c r="O737" s="40"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:P3"/>
+  <autoFilter ref="A3:P3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="99">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M267 M730:M733">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M267 M730:M733" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$M$15:$M$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N267 N730:N733">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N267 N730:N733" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$N$15:$N$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M261:M263 M265:M266">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M261:M263 M265:M266" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$M$16:$M$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N261:N263 N265:N266">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N261:N263 N265:N266" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>$N$16:$N$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N268 N424 N688:N691 N432:N435 N454 N550 N560:N562">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N268 N424 N688:N691 N432:N435 N454 N550 N560:N562" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>$N$12:$N$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M268 M554:M558">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M268 M554:M558" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>$M$13:$M$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N279 N269:N271 N724 N692">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N279 N269:N271 N724 N692" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>$N$9:$N$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M269 M552:M553">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M269 M552:M553" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>$M$10:$M$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M271 M724 M692">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M271 M724 M692" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>$M$9:$M$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M279">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M279" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>$M$9:$M$185</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M424 M432:M435 M454 M550 M560:M562">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M424 M432:M435 M454 M550 M560:M562" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>$M$12:$M$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N377:N423 N676:N685">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N377:N423 N676:N685" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>$N$54:$N$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M377:M423">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M377:M423" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>$M$54:$M$58</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N425:N431 N331:N338 N347">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N425:N431 N331:N338 N347" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>$N$18:$N$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M425:M431 M331:M338 M347">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M425:M431 M331:M338 M347" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>$M$18:$M$22</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M325:M330 M301:M303">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M325:M330 M301:M303" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>$M$83:$M$87</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N325:N330 N301:N303">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N325:N330 N301:N303" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>$N$83:$N$85</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N273">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N273" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>$N$189:$N$191</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M273">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M273" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>$M$189:$M$193</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M577:M578">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M577:M578" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>$L$10:$L$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N577:N578">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N577:N578" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>$M$10:$M$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M572:M576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M572:M576" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>$L$15:$L$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M571">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M571" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>$L$12:$L$23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N571">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N571" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>$M$12:$M$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N572:N576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N572:N576" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>$M$15:$M$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M570">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M570" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>$L$20:$L$24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N570">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N570" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>$M$20:$M$22</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M565:M569">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M565:M569" xr:uid="{00000000-0002-0000-0000-00001B000000}">
       <formula1>$L$22:$L$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N565:N569">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N565:N569" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>$M$22:$M$24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N564">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N564" xr:uid="{00000000-0002-0000-0000-00001D000000}">
       <formula1>$M$26:$M$28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M563">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M563" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>$L$27:$L$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N563">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N563" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>$M$27:$M$29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N339:N346">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N339:N346" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>$M$12:$M$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M339:M346">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M339:M346" xr:uid="{00000000-0002-0000-0000-000021000000}">
       <formula1>$L$12:$L$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M599:N601 M579:N595 M608:N630 M548:N549 M551 N8 M4:N7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M599:N601 M579:N595 M608:N630 M548:N549 M551 N8 M4:N7" xr:uid="{00000000-0002-0000-0000-000022000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M596:M598">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M596:M598" xr:uid="{00000000-0002-0000-0000-000023000000}">
       <formula1>$J$10:$J$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N596:N598">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N596:N598" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>$K$10:$K$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N264">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N264" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>$M$16:$M$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M264">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M264" xr:uid="{00000000-0002-0000-0000-000026000000}">
       <formula1>$L$16:$L$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N272">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N272" xr:uid="{00000000-0002-0000-0000-000027000000}">
       <formula1>$L$861:$L$865</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M564">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M564" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>$K$22:$K$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M734:M736 M559">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M734:M736 M559" xr:uid="{00000000-0002-0000-0000-000029000000}">
       <formula1>$M$11:$M$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N734:N736 N559">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N734:N736 N559" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>$N$11:$N$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M632">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M632" xr:uid="{00000000-0002-0000-0000-00002B000000}">
       <formula1>$K$12:$K$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N632">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N632" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>$L$12:$L$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N697:N716">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N697:N716" xr:uid="{00000000-0002-0000-0000-00002D000000}">
       <formula1>$N$24:$N$25</formula1>
     </dataValidation>
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O693:O696"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M693:M696">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O693:O696" xr:uid="{00000000-0002-0000-0000-00002E000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M693:M696" xr:uid="{00000000-0002-0000-0000-00002F000000}">
       <formula1>$M$13:$M$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N693:N696">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N693:N696" xr:uid="{00000000-0002-0000-0000-000030000000}">
       <formula1>$N$13:$N$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N639:N643">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N639:N643" xr:uid="{00000000-0002-0000-0000-000031000000}">
       <formula1>$N$57:$N$57</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M639:M643">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M639:M643" xr:uid="{00000000-0002-0000-0000-000032000000}">
       <formula1>$M$57:$M$59</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M662">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M662" xr:uid="{00000000-0002-0000-0000-000033000000}">
       <formula1>$M$30:$M$33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N662">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N662" xr:uid="{00000000-0002-0000-0000-000034000000}">
       <formula1>$N$30:$N$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M661">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M661" xr:uid="{00000000-0002-0000-0000-000035000000}">
       <formula1>$M$30:$M$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N661">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N661" xr:uid="{00000000-0002-0000-0000-000036000000}">
       <formula1>$N$30:$N$32</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M658">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M658" xr:uid="{00000000-0002-0000-0000-000037000000}">
       <formula1>$M$31:$M$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N658">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N658" xr:uid="{00000000-0002-0000-0000-000038000000}">
       <formula1>$N$31:$N$33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M657">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M657" xr:uid="{00000000-0002-0000-0000-000039000000}">
       <formula1>$M$32:$M$37</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N657">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N657" xr:uid="{00000000-0002-0000-0000-00003A000000}">
       <formula1>$N$32:$N$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M655">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M655" xr:uid="{00000000-0002-0000-0000-00003B000000}">
       <formula1>$M$34:$M$39</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N655">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N655" xr:uid="{00000000-0002-0000-0000-00003C000000}">
       <formula1>$N$34:$N$37</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M646">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M646" xr:uid="{00000000-0002-0000-0000-00003D000000}">
       <formula1>$M$35:$M$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N646">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N646" xr:uid="{00000000-0002-0000-0000-00003E000000}">
       <formula1>$N$35:$N$38</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M644 M659 M654 M648:M651">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M644 M659 M654 M648:M651" xr:uid="{00000000-0002-0000-0000-00003F000000}">
       <formula1>$M$53:$M$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N644 N659 N654 N648:N651">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N644 N659 N654 N648:N651" xr:uid="{00000000-0002-0000-0000-000040000000}">
       <formula1>$N$53:$N$55</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M652:M653 M663 M660 M645 M647 M656">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M652:M653 M663 M660 M645 M647 M656" xr:uid="{00000000-0002-0000-0000-000041000000}">
       <formula1>$M$33:$M$38</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N652:N653 N656 N647 N645 N660 N663">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N652:N653 N656 N647 N645 N660 N663" xr:uid="{00000000-0002-0000-0000-000042000000}">
       <formula1>$N$33:$N$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M668:M675">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M668:M675" xr:uid="{00000000-0002-0000-0000-000043000000}">
       <formula1>$M$55:$M$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N668:N675">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N668:N675" xr:uid="{00000000-0002-0000-0000-000044000000}">
       <formula1>$N$55:$N$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M676:M685">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M676:M685" xr:uid="{00000000-0002-0000-0000-000045000000}">
       <formula1>$M$54:$M$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M686:M687 M664:M667">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M686:M687 M664:M667" xr:uid="{00000000-0002-0000-0000-000046000000}">
       <formula1>$M$13:$M$23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N686:N687 N664:N667">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N686:N687 N664:N667" xr:uid="{00000000-0002-0000-0000-000047000000}">
       <formula1>$N$13:$N$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M688:M691">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M688:M691" xr:uid="{00000000-0002-0000-0000-000048000000}">
       <formula1>$M$12:$M$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N634:N638">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N634:N638" xr:uid="{00000000-0002-0000-0000-000049000000}">
       <formula1>$N$90:$N$91</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M634:M638">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M634:M638" xr:uid="{00000000-0002-0000-0000-00004A000000}">
       <formula1>$M$90:$M$93</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N633">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N633" xr:uid="{00000000-0002-0000-0000-00004B000000}">
       <formula1>$N$6:$N$90</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M633">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M633" xr:uid="{00000000-0002-0000-0000-00004C000000}">
       <formula1>$M$6:$M$92</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N631">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N631" xr:uid="{00000000-0002-0000-0000-00004D000000}">
       <formula1>$N$90:$N$92</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M631">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M631" xr:uid="{00000000-0002-0000-0000-00004E000000}">
       <formula1>$M$90:$M$94</formula1>
     </dataValidation>
-    <dataValidation imeMode="halfAlpha" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I725:K725 J728:K728 E725 I727:K727 P727 K726 K729:L729 P725 J630"/>
-    <dataValidation imeMode="hiragana" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F729 F726"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N717:N723">
+    <dataValidation imeMode="halfAlpha" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I725:K725 J728:K728 E725 I727:K727 P727 K726 K729:L729 P725 J630" xr:uid="{00000000-0002-0000-0000-00004F000000}"/>
+    <dataValidation imeMode="hiragana" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F729 F726" xr:uid="{00000000-0002-0000-0000-000050000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N717:N723" xr:uid="{00000000-0002-0000-0000-000051000000}">
       <formula1>$L$107:$L$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M717:M720 M723">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M717:M720 M723" xr:uid="{00000000-0002-0000-0000-000052000000}">
       <formula1>$K$107:$K$111</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N554:N558">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N554:N558" xr:uid="{00000000-0002-0000-0000-000053000000}">
       <formula1>$N$13:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N552:N553">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N552:N553" xr:uid="{00000000-0002-0000-0000-000054000000}">
       <formula1>$N$10:$N$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M486:M547">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M486:M547" xr:uid="{00000000-0002-0000-0000-000055000000}">
       <formula1>$M$70:$M$74</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N486:N547">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N486:N547" xr:uid="{00000000-0002-0000-0000-000056000000}">
       <formula1>$N$70:$N$72</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M437:M453">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M437:M453" xr:uid="{00000000-0002-0000-0000-000057000000}">
       <formula1>$M$142:$M$146</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N437:N453">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N437:N453" xr:uid="{00000000-0002-0000-0000-000058000000}">
       <formula1>$N$142:$N$144</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M436">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M436" xr:uid="{00000000-0002-0000-0000-000059000000}">
       <formula1>$K$145:$K$149</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N436">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N436" xr:uid="{00000000-0002-0000-0000-00005A000000}">
       <formula1>$L$145:$L$147</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M274:M277">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M274:M277" xr:uid="{00000000-0002-0000-0000-00005B000000}">
       <formula1>$M$188:$M$192</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N274:N277">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N274:N277" xr:uid="{00000000-0002-0000-0000-00005C000000}">
       <formula1>$N$188:$N$190</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M278">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M278" xr:uid="{00000000-0002-0000-0000-00005D000000}">
       <formula1>$L$188:$L$192</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N278">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N278" xr:uid="{00000000-0002-0000-0000-00005E000000}">
       <formula1>$M$188:$M$190</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8" xr:uid="{00000000-0002-0000-0000-00005F000000}">
       <formula1>$M$738:$M$738</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="N9:N260">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="N9:N260" xr:uid="{00000000-0002-0000-0000-000060000000}">
       <formula1>$N$737:$N$737</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M260">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M260" xr:uid="{00000000-0002-0000-0000-000061000000}">
       <formula1>$M$737:$M$737</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M721:M722">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M721:M722" xr:uid="{00000000-0002-0000-0000-000062000000}">
       <formula1>$M$109:$M$113</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.59055118110236227" bottom="0.31496062992125984" header="0.11811023622047245" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L
 </oddHeader>

</xml_diff>